<commit_message>
Updated with Models data
</commit_message>
<xml_diff>
--- a/Assignments/Assignment 4.xlsx
+++ b/Assignments/Assignment 4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop\Data Analyst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop\Data Analyst\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04F1707-9FF4-4CFB-B3E8-F0551852E1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FC50C6-56E5-49BB-8A8E-43B15872AD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{1E8CDBDE-CDCC-4E41-9F59-98A0FDD1CAA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{1E8CDBDE-CDCC-4E41-9F59-98A0FDD1CAA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment_4_Navigation" sheetId="3" r:id="rId1"/>
@@ -1915,7 +1915,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2302,26 +2302,29 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="1" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2840,7 +2843,7 @@
   </sheetPr>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="132" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="132" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -2897,7 +2900,7 @@
       </c>
       <c r="I2" s="129">
         <f ca="1">RANDBETWEEN(H2,G2)</f>
-        <v>699</v>
+        <v>747</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2911,7 +2914,7 @@
       </c>
       <c r="I3" s="129">
         <f ca="1">RANDBETWEEN(G3,H3)</f>
-        <v>139</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2935,7 +2938,7 @@
       </c>
       <c r="I4" s="129">
         <f ca="1">RANDBETWEEN(G4,H4)</f>
-        <v>650600</v>
+        <v>175840</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2961,7 +2964,7 @@
       </c>
       <c r="I5" s="129">
         <f t="shared" ref="I5:I7" ca="1" si="0">RANDBETWEEN(H5,G5)</f>
-        <v>4938</v>
+        <v>3264</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2980,7 +2983,7 @@
       </c>
       <c r="I6" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>3740</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3005,7 +3008,7 @@
       </c>
       <c r="I7" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>473682</v>
+        <v>86199</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3080,7 +3083,7 @@
       </c>
       <c r="I11" s="129">
         <f ca="1">RANDBETWEEN(G11,H11)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3140,7 +3143,7 @@
       </c>
       <c r="I15" s="129">
         <f ca="1">RANDBETWEEN(G15,H15)</f>
-        <v>9132</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3419,17 +3422,17 @@
         <f>POWER(A39,3)</f>
         <v>216</v>
       </c>
-      <c r="D39" s="138" t="s">
+      <c r="D39" s="135" t="s">
         <v>361</v>
       </c>
-      <c r="E39" s="138"/>
+      <c r="E39" s="135"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D40" s="134">
+      <c r="D40" s="136">
         <f ca="1">RAND()</f>
-        <v>0.13958514086217189</v>
-      </c>
-      <c r="E40" s="134"/>
+        <v>0.89620612957243107</v>
+      </c>
+      <c r="E40" s="136"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="35" t="s">
@@ -3438,11 +3441,11 @@
       <c r="B41" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="D41" s="134">
+      <c r="D41" s="136">
         <f t="shared" ref="D41:D45" ca="1" si="3">RAND()</f>
-        <v>0.35010446885178503</v>
-      </c>
-      <c r="E41" s="134"/>
+        <v>0.24410467657076429</v>
+      </c>
+      <c r="E41" s="136"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="122">
@@ -3452,18 +3455,18 @@
         <f>INT(A42)</f>
         <v>76</v>
       </c>
-      <c r="D42" s="134">
+      <c r="D42" s="136">
         <f t="shared" ca="1" si="3"/>
-        <v>0.9506578428106699</v>
-      </c>
-      <c r="E42" s="134"/>
+        <v>0.92166225461834572</v>
+      </c>
+      <c r="E42" s="136"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D43" s="134">
+      <c r="D43" s="136">
         <f t="shared" ca="1" si="3"/>
-        <v>0.11473930468528815</v>
-      </c>
-      <c r="E43" s="134"/>
+        <v>0.55165947557042971</v>
+      </c>
+      <c r="E43" s="136"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="35" t="s">
@@ -3472,11 +3475,11 @@
       <c r="B44" s="35" t="s">
         <v>342</v>
       </c>
-      <c r="D44" s="134">
+      <c r="D44" s="136">
         <f t="shared" ca="1" si="3"/>
-        <v>7.938632889712971E-3</v>
-      </c>
-      <c r="E44" s="134"/>
+        <v>0.69448667413198484</v>
+      </c>
+      <c r="E44" s="136"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="125">
@@ -3486,11 +3489,11 @@
         <f>INT(A45)</f>
         <v>45</v>
       </c>
-      <c r="D45" s="134">
+      <c r="D45" s="136">
         <f t="shared" ca="1" si="3"/>
-        <v>0.46006948062396158</v>
-      </c>
-      <c r="E45" s="134"/>
+        <v>0.27461562398627748</v>
+      </c>
+      <c r="E45" s="136"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
@@ -3512,11 +3515,11 @@
         <f>INT(A48)</f>
         <v>76</v>
       </c>
-      <c r="D48" s="135">
+      <c r="D48" s="134">
         <f ca="1">RAND()/100</f>
-        <v>9.1164669997768064E-4</v>
-      </c>
-      <c r="E48" s="135"/>
+        <v>8.6829645976143413E-3</v>
+      </c>
+      <c r="E48" s="134"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="124">
@@ -3526,11 +3529,11 @@
         <f t="shared" ref="B49:B57" si="4">INT(A49)</f>
         <v>56</v>
       </c>
-      <c r="D49" s="135">
+      <c r="D49" s="134">
         <f t="shared" ref="D49:D53" ca="1" si="5">RAND()/100</f>
-        <v>5.7641839988107832E-3</v>
-      </c>
-      <c r="E49" s="135"/>
+        <v>4.8044084420447841E-3</v>
+      </c>
+      <c r="E49" s="134"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="124">
@@ -3540,11 +3543,11 @@
         <f t="shared" si="4"/>
         <v>99</v>
       </c>
-      <c r="D50" s="135">
+      <c r="D50" s="134">
         <f t="shared" ca="1" si="5"/>
-        <v>9.5035568220527052E-3</v>
-      </c>
-      <c r="E50" s="135"/>
+        <v>2.3086289843215735E-3</v>
+      </c>
+      <c r="E50" s="134"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="124">
@@ -3554,11 +3557,11 @@
         <f t="shared" si="4"/>
         <v>513</v>
       </c>
-      <c r="D51" s="135">
+      <c r="D51" s="134">
         <f t="shared" ca="1" si="5"/>
-        <v>8.6880117475818255E-7</v>
-      </c>
-      <c r="E51" s="135"/>
+        <v>7.0676417843931463E-3</v>
+      </c>
+      <c r="E51" s="134"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="124">
@@ -3568,11 +3571,11 @@
         <f t="shared" si="4"/>
         <v>823</v>
       </c>
-      <c r="D52" s="135">
+      <c r="D52" s="134">
         <f t="shared" ca="1" si="5"/>
-        <v>9.7111145420270377E-3</v>
-      </c>
-      <c r="E52" s="135"/>
+        <v>4.6765671146995931E-3</v>
+      </c>
+      <c r="E52" s="134"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="124">
@@ -3582,11 +3585,11 @@
         <f t="shared" si="4"/>
         <v>46</v>
       </c>
-      <c r="D53" s="135">
+      <c r="D53" s="134">
         <f t="shared" ca="1" si="5"/>
-        <v>3.4254641649946183E-3</v>
-      </c>
-      <c r="E53" s="135"/>
+        <v>4.4818057775446599E-3</v>
+      </c>
+      <c r="E53" s="134"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="124">
@@ -3614,10 +3617,10 @@
         <f t="shared" si="4"/>
         <v>135</v>
       </c>
-      <c r="D56" s="136" t="s">
+      <c r="D56" s="138" t="s">
         <v>363</v>
       </c>
-      <c r="E56" s="136"/>
+      <c r="E56" s="138"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="124">
@@ -3627,49 +3630,58 @@
         <f t="shared" si="4"/>
         <v>2364</v>
       </c>
-      <c r="D57" s="134">
+      <c r="D57" s="136">
         <f ca="1">RAND()*100</f>
-        <v>34.794469367763448</v>
-      </c>
-      <c r="E57" s="134"/>
+        <v>63.822043771953261</v>
+      </c>
+      <c r="E57" s="136"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D58" s="134">
+      <c r="D58" s="136">
         <f t="shared" ref="D58:D62" ca="1" si="6">RAND()*100</f>
-        <v>14.372276123596484</v>
-      </c>
-      <c r="E58" s="134"/>
+        <v>1.5217409465220544</v>
+      </c>
+      <c r="E58" s="136"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D59" s="134">
+      <c r="D59" s="136">
         <f t="shared" ca="1" si="6"/>
-        <v>24.143737613404902</v>
-      </c>
-      <c r="E59" s="134"/>
+        <v>80.417623268622648</v>
+      </c>
+      <c r="E59" s="136"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D60" s="134">
+      <c r="D60" s="136">
         <f t="shared" ca="1" si="6"/>
-        <v>8.2770852738734639</v>
-      </c>
-      <c r="E60" s="134"/>
+        <v>20.463465857572473</v>
+      </c>
+      <c r="E60" s="136"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D61" s="134">
+      <c r="D61" s="136">
         <f t="shared" ca="1" si="6"/>
-        <v>28.526890043018305</v>
-      </c>
-      <c r="E61" s="134"/>
+        <v>99.066859694734219</v>
+      </c>
+      <c r="E61" s="136"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D62" s="134">
+      <c r="D62" s="136">
         <f t="shared" ca="1" si="6"/>
-        <v>73.155640146372519</v>
-      </c>
-      <c r="E62" s="134"/>
+        <v>23.070374039508433</v>
+      </c>
+      <c r="E62" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="D40:E40"/>
@@ -3682,15 +3694,6 @@
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3805,13 +3808,13 @@
         <f>SUMIF(TBL_SALES[BRAND_NAME],TBL_SALES[[#This Row],[BRAND_NAME]],TBL_SALES[SALES_AMOUNT])</f>
         <v>3447703</v>
       </c>
-      <c r="Q2" s="140" t="s">
+      <c r="Q2" s="139" t="s">
         <v>226</v>
       </c>
-      <c r="R2" s="140"/>
-      <c r="S2" s="140"/>
-      <c r="T2" s="140"/>
-      <c r="U2" s="140"/>
+      <c r="R2" s="139"/>
+      <c r="S2" s="139"/>
+      <c r="T2" s="139"/>
+      <c r="U2" s="139"/>
       <c r="Y2" s="19" t="s">
         <v>243</v>
       </c>
@@ -3867,14 +3870,14 @@
         <f>SUMIF(TBL_SALES[BRAND_NAME],TBL_SALES[[#This Row],[BRAND_NAME]],TBL_SALES[SALES_AMOUNT])</f>
         <v>3447703</v>
       </c>
-      <c r="Q3" s="139">
+      <c r="Q3" s="140">
         <f>SUMIFS(E:E,B:B,B2,H:H,TBL_SALES[[#This Row],[STATE]])</f>
         <v>103</v>
       </c>
-      <c r="R3" s="139"/>
-      <c r="S3" s="139"/>
-      <c r="T3" s="139"/>
-      <c r="U3" s="139"/>
+      <c r="R3" s="140"/>
+      <c r="S3" s="140"/>
+      <c r="T3" s="140"/>
+      <c r="U3" s="140"/>
       <c r="Y3" s="22" t="s">
         <v>11</v>
       </c>
@@ -3936,11 +3939,11 @@
       <c r="M4" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="Q4" s="139"/>
-      <c r="R4" s="139"/>
-      <c r="S4" s="139"/>
-      <c r="T4" s="139"/>
-      <c r="U4" s="139"/>
+      <c r="Q4" s="140"/>
+      <c r="R4" s="140"/>
+      <c r="S4" s="140"/>
+      <c r="T4" s="140"/>
+      <c r="U4" s="140"/>
       <c r="Y4" s="23" t="s">
         <v>20</v>
       </c>
@@ -4003,11 +4006,11 @@
         <f>_xlfn.MINIFS(TBL_SALES[QUANTITY],TBL_SALES[PRODUCT_CTG],"Laptop",TBL_SALES[BRAND_NAME],"HP",TBL_SALES[STATE],"Karnataka")</f>
         <v>1</v>
       </c>
-      <c r="Q5" s="139"/>
-      <c r="R5" s="139"/>
-      <c r="S5" s="139"/>
-      <c r="T5" s="139"/>
-      <c r="U5" s="139"/>
+      <c r="Q5" s="140"/>
+      <c r="R5" s="140"/>
+      <c r="S5" s="140"/>
+      <c r="T5" s="140"/>
+      <c r="U5" s="140"/>
       <c r="Y5" s="24" t="s">
         <v>23</v>
       </c>
@@ -4183,13 +4186,13 @@
         <v>5071935</v>
       </c>
       <c r="O8" s="5"/>
-      <c r="Q8" s="140" t="s">
+      <c r="Q8" s="139" t="s">
         <v>227</v>
       </c>
-      <c r="R8" s="140"/>
-      <c r="S8" s="140"/>
-      <c r="T8" s="140"/>
-      <c r="U8" s="140"/>
+      <c r="R8" s="139"/>
+      <c r="S8" s="139"/>
+      <c r="T8" s="139"/>
+      <c r="U8" s="139"/>
       <c r="Y8" s="23" t="s">
         <v>47</v>
       </c>
@@ -4248,14 +4251,14 @@
         <f>SUMIF(TBL_SALES[BRAND_NAME],TBL_SALES[[#This Row],[BRAND_NAME]],TBL_SALES[SALES_AMOUNT])</f>
         <v>5071935</v>
       </c>
-      <c r="Q9" s="139">
+      <c r="Q9" s="140">
         <f>SUMIFS(E:E,B:B,B102,H:H,H5)</f>
         <v>50</v>
       </c>
-      <c r="R9" s="139"/>
-      <c r="S9" s="139"/>
-      <c r="T9" s="139"/>
-      <c r="U9" s="139"/>
+      <c r="R9" s="140"/>
+      <c r="S9" s="140"/>
+      <c r="T9" s="140"/>
+      <c r="U9" s="140"/>
       <c r="Y9" s="23" t="s">
         <v>145</v>
       </c>
@@ -4317,11 +4320,11 @@
       <c r="O10" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="Q10" s="139"/>
-      <c r="R10" s="139"/>
-      <c r="S10" s="139"/>
-      <c r="T10" s="139"/>
-      <c r="U10" s="139"/>
+      <c r="Q10" s="140"/>
+      <c r="R10" s="140"/>
+      <c r="S10" s="140"/>
+      <c r="T10" s="140"/>
+      <c r="U10" s="140"/>
       <c r="Y10" s="24" t="s">
         <v>148</v>
       </c>
@@ -4384,11 +4387,11 @@
         <f>AVERAGEIFS(F:F,B:B,B4,H:H,H6)</f>
         <v>83348.192307692312</v>
       </c>
-      <c r="Q11" s="139"/>
-      <c r="R11" s="139"/>
-      <c r="S11" s="139"/>
-      <c r="T11" s="139"/>
-      <c r="U11" s="139"/>
+      <c r="Q11" s="140"/>
+      <c r="R11" s="140"/>
+      <c r="S11" s="140"/>
+      <c r="T11" s="140"/>
+      <c r="U11" s="140"/>
       <c r="Y11" s="23" t="s">
         <v>151</v>
       </c>
@@ -4566,13 +4569,13 @@
       <c r="O14" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="Q14" s="140" t="s">
+      <c r="Q14" s="139" t="s">
         <v>228</v>
       </c>
-      <c r="R14" s="140"/>
-      <c r="S14" s="140"/>
-      <c r="T14" s="140"/>
-      <c r="U14" s="140"/>
+      <c r="R14" s="139"/>
+      <c r="S14" s="139"/>
+      <c r="T14" s="139"/>
+      <c r="U14" s="139"/>
       <c r="Y14" s="23" t="s">
         <v>161</v>
       </c>
@@ -4628,14 +4631,14 @@
         <f>COUNTA(TBL_SALES[SALEID])</f>
         <v>160</v>
       </c>
-      <c r="Q15" s="139">
+      <c r="Q15" s="140">
         <f>AVERAGEIFS(F:F,C:C,C8)</f>
         <v>82926.350000000006</v>
       </c>
-      <c r="R15" s="139"/>
-      <c r="S15" s="139"/>
-      <c r="T15" s="139"/>
-      <c r="U15" s="139"/>
+      <c r="R15" s="140"/>
+      <c r="S15" s="140"/>
+      <c r="T15" s="140"/>
+      <c r="U15" s="140"/>
       <c r="Y15" s="23" t="s">
         <v>167</v>
       </c>
@@ -4690,11 +4693,11 @@
       <c r="M16" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="Q16" s="139"/>
-      <c r="R16" s="139"/>
-      <c r="S16" s="139"/>
-      <c r="T16" s="139"/>
-      <c r="U16" s="139"/>
+      <c r="Q16" s="140"/>
+      <c r="R16" s="140"/>
+      <c r="S16" s="140"/>
+      <c r="T16" s="140"/>
+      <c r="U16" s="140"/>
       <c r="Y16" s="23" t="s">
         <v>171</v>
       </c>
@@ -4750,11 +4753,11 @@
         <f>_xlfn.MINIFS(F:F,B:B,B129)</f>
         <v>13403</v>
       </c>
-      <c r="Q17" s="139"/>
-      <c r="R17" s="139"/>
-      <c r="S17" s="139"/>
-      <c r="T17" s="139"/>
-      <c r="U17" s="139"/>
+      <c r="Q17" s="140"/>
+      <c r="R17" s="140"/>
+      <c r="S17" s="140"/>
+      <c r="T17" s="140"/>
+      <c r="U17" s="140"/>
       <c r="Y17" s="25" t="s">
         <v>181</v>
       </c>
@@ -4809,11 +4812,11 @@
       <c r="O18" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="Q18" s="139"/>
-      <c r="R18" s="139"/>
-      <c r="S18" s="139"/>
-      <c r="T18" s="139"/>
-      <c r="U18" s="139"/>
+      <c r="Q18" s="140"/>
+      <c r="R18" s="140"/>
+      <c r="S18" s="140"/>
+      <c r="T18" s="140"/>
+      <c r="U18" s="140"/>
       <c r="Y18" s="21" t="s">
         <v>189</v>
       </c>
@@ -4943,13 +4946,13 @@
         <f>SUMIF(TBL_SALES[BRAND_NAME],TBL_SALES[[#This Row],[BRAND_NAME]],TBL_SALES[SALES_AMOUNT])</f>
         <v>2939163</v>
       </c>
-      <c r="Q21" s="140" t="s">
+      <c r="Q21" s="139" t="s">
         <v>229</v>
       </c>
-      <c r="R21" s="140"/>
-      <c r="S21" s="140"/>
-      <c r="T21" s="140"/>
-      <c r="U21" s="140"/>
+      <c r="R21" s="139"/>
+      <c r="S21" s="139"/>
+      <c r="T21" s="139"/>
+      <c r="U21" s="139"/>
       <c r="Y21" s="34" t="s">
         <v>243</v>
       </c>
@@ -5002,14 +5005,14 @@
       <c r="O22" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="Q22" s="139">
+      <c r="Q22" s="140">
         <f>AVERAGEIFS(E:E,B:B,B2)</f>
         <v>3.1</v>
       </c>
-      <c r="R22" s="139"/>
-      <c r="S22" s="139"/>
-      <c r="T22" s="139"/>
-      <c r="U22" s="139"/>
+      <c r="R22" s="140"/>
+      <c r="S22" s="140"/>
+      <c r="T22" s="140"/>
+      <c r="U22" s="140"/>
       <c r="Y22" s="18" t="s">
         <v>11</v>
       </c>
@@ -5065,11 +5068,11 @@
         <f>COUNTBLANK(TBL_SALES[STATE])</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="139"/>
-      <c r="R23" s="139"/>
-      <c r="S23" s="139"/>
-      <c r="T23" s="139"/>
-      <c r="U23" s="139"/>
+      <c r="Q23" s="140"/>
+      <c r="R23" s="140"/>
+      <c r="S23" s="140"/>
+      <c r="T23" s="140"/>
+      <c r="U23" s="140"/>
       <c r="Y23" s="17" t="s">
         <v>20</v>
       </c>
@@ -5121,11 +5124,11 @@
         <f>SUMIF(TBL_SALES[BRAND_NAME],TBL_SALES[[#This Row],[BRAND_NAME]],TBL_SALES[SALES_AMOUNT])</f>
         <v>3447703</v>
       </c>
-      <c r="Q24" s="139"/>
-      <c r="R24" s="139"/>
-      <c r="S24" s="139"/>
-      <c r="T24" s="139"/>
-      <c r="U24" s="139"/>
+      <c r="Q24" s="140"/>
+      <c r="R24" s="140"/>
+      <c r="S24" s="140"/>
+      <c r="T24" s="140"/>
+      <c r="U24" s="140"/>
       <c r="Y24" s="18" t="s">
         <v>23</v>
       </c>
@@ -5180,11 +5183,11 @@
       <c r="O25" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="Q25" s="139"/>
-      <c r="R25" s="139"/>
-      <c r="S25" s="139"/>
-      <c r="T25" s="139"/>
-      <c r="U25" s="139"/>
+      <c r="Q25" s="140"/>
+      <c r="R25" s="140"/>
+      <c r="S25" s="140"/>
+      <c r="T25" s="140"/>
+      <c r="U25" s="140"/>
       <c r="Y25" s="18" t="s">
         <v>30</v>
       </c>
@@ -5291,13 +5294,13 @@
         <f>SUMIF(TBL_SALES[BRAND_NAME],TBL_SALES[[#This Row],[BRAND_NAME]],TBL_SALES[SALES_AMOUNT])</f>
         <v>4627368</v>
       </c>
-      <c r="Q27" s="140" t="s">
+      <c r="Q27" s="139" t="s">
         <v>230</v>
       </c>
-      <c r="R27" s="140"/>
-      <c r="S27" s="140"/>
-      <c r="T27" s="140"/>
-      <c r="U27" s="140"/>
+      <c r="R27" s="139"/>
+      <c r="S27" s="139"/>
+      <c r="T27" s="139"/>
+      <c r="U27" s="139"/>
       <c r="Y27" s="17" t="s">
         <v>47</v>
       </c>
@@ -5345,14 +5348,14 @@
       <c r="M28" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="Q28" s="139">
+      <c r="Q28" s="140">
         <f>AVERAGEIFS(TBL_SALES[QUANTITY],TBL_SALES[PRODUCT_CTG],B153)</f>
         <v>2.7166666666666668</v>
       </c>
-      <c r="R28" s="139"/>
-      <c r="S28" s="139"/>
-      <c r="T28" s="139"/>
-      <c r="U28" s="139"/>
+      <c r="R28" s="140"/>
+      <c r="S28" s="140"/>
+      <c r="T28" s="140"/>
+      <c r="U28" s="140"/>
       <c r="Y28" s="17" t="s">
         <v>145</v>
       </c>
@@ -5404,11 +5407,11 @@
       <c r="O29" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="Q29" s="139"/>
-      <c r="R29" s="139"/>
-      <c r="S29" s="139"/>
-      <c r="T29" s="139"/>
-      <c r="U29" s="139"/>
+      <c r="Q29" s="140"/>
+      <c r="R29" s="140"/>
+      <c r="S29" s="140"/>
+      <c r="T29" s="140"/>
+      <c r="U29" s="140"/>
       <c r="Y29" s="18" t="s">
         <v>148</v>
       </c>
@@ -5457,11 +5460,11 @@
         <f>COUNTIFS(TBL_SALES[DATE], "&gt;=" &amp; DATE(2025,1,1), TBL_SALES[DATE], "&lt;=" &amp; DATE(2025,12,31))</f>
         <v>91</v>
       </c>
-      <c r="Q30" s="139"/>
-      <c r="R30" s="139"/>
-      <c r="S30" s="139"/>
-      <c r="T30" s="139"/>
-      <c r="U30" s="139"/>
+      <c r="Q30" s="140"/>
+      <c r="R30" s="140"/>
+      <c r="S30" s="140"/>
+      <c r="T30" s="140"/>
+      <c r="U30" s="140"/>
       <c r="Y30" s="17" t="s">
         <v>151</v>
       </c>
@@ -5506,11 +5509,11 @@
         <f>SUMIF(TBL_SALES[BRAND_NAME],TBL_SALES[[#This Row],[BRAND_NAME]],TBL_SALES[SALES_AMOUNT])</f>
         <v>2863185</v>
       </c>
-      <c r="Q31" s="139"/>
-      <c r="R31" s="139"/>
-      <c r="S31" s="139"/>
-      <c r="T31" s="139"/>
-      <c r="U31" s="139"/>
+      <c r="Q31" s="140"/>
+      <c r="R31" s="140"/>
+      <c r="S31" s="140"/>
+      <c r="T31" s="140"/>
+      <c r="U31" s="140"/>
       <c r="Y31" s="18" t="s">
         <v>154</v>
       </c>
@@ -10408,16 +10411,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="Q22:U25"/>
+    <mergeCell ref="Q21:U21"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="Q28:U31"/>
+    <mergeCell ref="Q3:U5"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="Q8:U8"/>
     <mergeCell ref="Q9:U11"/>
     <mergeCell ref="Q14:U14"/>
     <mergeCell ref="Q15:U18"/>
-    <mergeCell ref="Q22:U25"/>
-    <mergeCell ref="Q21:U21"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="Q28:U31"/>
-    <mergeCell ref="Q3:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -10433,8 +10436,8 @@
   </sheetPr>
   <dimension ref="A1:AC161"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F151" sqref="F151"/>
+    <sheetView tabSelected="1" topLeftCell="R14" zoomScale="115" workbookViewId="0">
+      <selection activeCell="Y31" sqref="Y31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10446,7 +10449,7 @@
     <col min="16" max="16" width="5.7109375" style="40" customWidth="1"/>
     <col min="17" max="17" width="32" style="40" customWidth="1"/>
     <col min="18" max="18" width="6.140625" style="40" customWidth="1"/>
-    <col min="19" max="19" width="29" style="40" customWidth="1"/>
+    <col min="19" max="19" width="36.5703125" style="40" customWidth="1"/>
     <col min="20" max="20" width="7.28515625" style="40" customWidth="1"/>
     <col min="21" max="21" width="34.5703125" style="40" customWidth="1"/>
     <col min="22" max="22" width="27.28515625" style="40" customWidth="1"/>
@@ -12039,9 +12042,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>ACER --&gt; Aspire 5</v>
       </c>
-      <c r="S24" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1023  Vijayawada  45533</v>
+      <c r="S24" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1023  Vijayawada  29-08-2024</v>
       </c>
       <c r="U24" s="51" t="s">
         <v>286</v>
@@ -12106,9 +12109,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>DELL --&gt; Inspiron 15</v>
       </c>
-      <c r="S25" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1024  Chennai  45486</v>
+      <c r="S25" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1024  Chennai  13-07-2024</v>
       </c>
       <c r="U25" s="51" t="s">
         <v>286</v>
@@ -12166,9 +12169,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>ACER --&gt; Predator Helios</v>
       </c>
-      <c r="S26" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1025  Trivandrum  45659</v>
+      <c r="S26" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1025  Trivandrum  02-01-2025</v>
       </c>
       <c r="U26" s="51" t="s">
         <v>286</v>
@@ -12226,9 +12229,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>MSI --&gt; GF63 Thin</v>
       </c>
-      <c r="S27" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1026  Chennai  45305</v>
+      <c r="S27" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1026  Chennai  14-01-2024</v>
       </c>
       <c r="U27" s="51" t="s">
         <v>286</v>
@@ -12286,9 +12289,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>ASUS --&gt; ROG Zephyrus</v>
       </c>
-      <c r="S28" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1027  Visakhapatnam  45823</v>
+      <c r="S28" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1027  Visakhapatnam  15-06-2025</v>
       </c>
       <c r="U28" s="51" t="s">
         <v>286</v>
@@ -12346,9 +12349,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>ASUS --&gt; Vivobook 15</v>
       </c>
-      <c r="S29" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1028  Vijayawada  45605</v>
+      <c r="S29" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1028  Vijayawada  09-11-2024</v>
       </c>
       <c r="U29" s="51" t="s">
         <v>286</v>
@@ -12406,9 +12409,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>ASUS --&gt; ROG Zephyrus</v>
       </c>
-      <c r="S30" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1029  Hyderabad  45400</v>
+      <c r="S30" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1029  Hyderabad  18-04-2024</v>
       </c>
       <c r="U30" s="51" t="s">
         <v>286</v>
@@ -12466,9 +12469,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>LENOVO --&gt; ThinkPad E14</v>
       </c>
-      <c r="S31" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1030  Chennai  45372</v>
+      <c r="S31" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1030  Chennai  21-03-2024</v>
       </c>
       <c r="U31" s="51" t="s">
         <v>286</v>
@@ -12526,9 +12529,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>ASUS --&gt; ROG Zephyrus</v>
       </c>
-      <c r="S32" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1031  Vijayawada  45562</v>
+      <c r="S32" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1031  Vijayawada  27-09-2024</v>
       </c>
       <c r="U32" s="51" t="s">
         <v>286</v>
@@ -12586,9 +12589,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>ASUS --&gt; Vivobook 15</v>
       </c>
-      <c r="S33" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1032  Coimbatore  45954</v>
+      <c r="S33" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1032  Coimbatore  24-10-2025</v>
       </c>
       <c r="U33" s="51" t="s">
         <v>286</v>
@@ -12646,9 +12649,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>HP --&gt; Pavilion 14</v>
       </c>
-      <c r="S34" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1033  Chennai  45522</v>
+      <c r="S34" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1033  Chennai  18-08-2024</v>
       </c>
       <c r="U34" s="51" t="s">
         <v>286</v>
@@ -12706,9 +12709,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>MSI --&gt; GF63 Thin</v>
       </c>
-      <c r="S35" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1034  Chennai  45403</v>
+      <c r="S35" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1034  Chennai  21-04-2024</v>
       </c>
       <c r="U35" s="51" t="s">
         <v>286</v>
@@ -12766,9 +12769,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>LENOVO --&gt; ThinkPad E14</v>
       </c>
-      <c r="S36" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1035  Hyderabad  45686</v>
+      <c r="S36" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1035  Hyderabad  29-01-2025</v>
       </c>
       <c r="U36" s="51" t="s">
         <v>286</v>
@@ -12826,9 +12829,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>HP --&gt; Pavilion 14</v>
       </c>
-      <c r="S37" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1036  Vijayawada  45486</v>
+      <c r="S37" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1036  Vijayawada  13-07-2024</v>
       </c>
       <c r="U37" s="51" t="s">
         <v>286</v>
@@ -12886,9 +12889,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>ASUS --&gt; Vivobook 15</v>
       </c>
-      <c r="S38" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1037  Visakhapatnam  45732</v>
+      <c r="S38" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1037  Visakhapatnam  16-03-2025</v>
       </c>
       <c r="U38" s="51" t="s">
         <v>286</v>
@@ -12946,9 +12949,9 @@
         <f>TBL_SALES3[BRAND_NAME]&amp;" --&gt; "&amp;TBL_SALES3[PRODUCT_NAME]</f>
         <v>ACER --&gt; Predator Helios</v>
       </c>
-      <c r="S39" s="51" t="str">
-        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TBL_SALES3[DATE])</f>
-        <v>S1038  Visakhapatnam  45554</v>
+      <c r="S39" s="141" t="str">
+        <f>CONCATENATE(TBL_SALES3[SALEID],"  ",TBL_SALES3[CITY],"  ",TEXT(TBL_SALES3[DATE],"dd-mm-yyyy"))</f>
+        <v>S1038  Visakhapatnam  19-09-2024</v>
       </c>
       <c r="U39" s="51" t="s">
         <v>286</v>

</xml_diff>